<commit_message>
Po createing with image
</commit_message>
<xml_diff>
--- a/Documents/March_2024/New_database_layout.xlsx
+++ b/Documents/March_2024/New_database_layout.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\SALINDA SANDARUWAN\SIBA_Dynamics\SIBA-Inventory-new-requirements\New_requirements_inventory\Documents\March_2024\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F74A4E02-51BB-46E9-BFDA-C7F0FC96F529}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A1940930-617B-4E76-A729-D6131FE7D0F8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -275,7 +275,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -285,6 +285,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FF00B0F0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF00B050"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -316,7 +322,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -337,6 +343,8 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -617,10 +625,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="B2:N81"/>
+  <dimension ref="A2:N81"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A59" workbookViewId="0">
-      <selection activeCell="C75" sqref="C75"/>
+    <sheetView tabSelected="1" topLeftCell="A67" workbookViewId="0">
+      <selection activeCell="C78" sqref="C78"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -640,12 +648,13 @@
     <col min="17" max="17" width="9.88671875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:14" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A2" s="10"/>
       <c r="B2" s="9" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="2:14" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:14" x14ac:dyDescent="0.3">
       <c r="B3" s="2" t="s">
         <v>1</v>
       </c>
@@ -668,7 +677,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="4" spans="2:14" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:14" x14ac:dyDescent="0.3">
       <c r="B4" s="5">
         <v>1</v>
       </c>
@@ -681,7 +690,7 @@
       <c r="G4" s="3"/>
       <c r="H4" s="3"/>
     </row>
-    <row r="5" spans="2:14" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:14" x14ac:dyDescent="0.3">
       <c r="B5" s="5">
         <v>2</v>
       </c>
@@ -703,7 +712,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="6" spans="2:14" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:14" x14ac:dyDescent="0.3">
       <c r="B6" s="5">
         <v>3</v>
       </c>
@@ -722,7 +731,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="7" spans="2:14" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:14" x14ac:dyDescent="0.3">
       <c r="B7" s="5">
         <v>4</v>
       </c>
@@ -735,7 +744,7 @@
       <c r="G7" s="3"/>
       <c r="H7" s="3"/>
     </row>
-    <row r="8" spans="2:14" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:14" x14ac:dyDescent="0.3">
       <c r="B8" s="5">
         <v>5</v>
       </c>
@@ -748,7 +757,7 @@
       <c r="G8" s="3"/>
       <c r="H8" s="3"/>
     </row>
-    <row r="9" spans="2:14" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:14" x14ac:dyDescent="0.3">
       <c r="B9" s="5">
         <v>6</v>
       </c>
@@ -761,7 +770,7 @@
       <c r="G9" s="3"/>
       <c r="H9" s="3"/>
     </row>
-    <row r="10" spans="2:14" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:14" x14ac:dyDescent="0.3">
       <c r="B10" s="5">
         <v>7</v>
       </c>
@@ -774,7 +783,7 @@
       <c r="G10" s="3"/>
       <c r="H10" s="3"/>
     </row>
-    <row r="11" spans="2:14" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:14" x14ac:dyDescent="0.3">
       <c r="B11" s="5">
         <v>8</v>
       </c>
@@ -787,7 +796,7 @@
       <c r="G11" s="3"/>
       <c r="H11" s="3"/>
     </row>
-    <row r="12" spans="2:14" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:14" x14ac:dyDescent="0.3">
       <c r="B12" s="5">
         <v>9</v>
       </c>
@@ -800,7 +809,7 @@
       <c r="G12" s="3"/>
       <c r="H12" s="3"/>
     </row>
-    <row r="13" spans="2:14" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:14" x14ac:dyDescent="0.3">
       <c r="B13" s="5">
         <v>10</v>
       </c>
@@ -813,7 +822,7 @@
       <c r="G13" s="3"/>
       <c r="H13" s="3"/>
     </row>
-    <row r="14" spans="2:14" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:14" x14ac:dyDescent="0.3">
       <c r="B14" s="5">
         <v>11</v>
       </c>
@@ -826,7 +835,7 @@
       <c r="G14" s="3"/>
       <c r="H14" s="3"/>
     </row>
-    <row r="15" spans="2:14" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:14" x14ac:dyDescent="0.3">
       <c r="B15" s="5">
         <v>12</v>
       </c>
@@ -839,7 +848,7 @@
       <c r="G15" s="3"/>
       <c r="H15" s="3"/>
     </row>
-    <row r="16" spans="2:14" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:14" x14ac:dyDescent="0.3">
       <c r="B16" s="5">
         <v>13</v>
       </c>
@@ -852,7 +861,7 @@
       <c r="G16" s="3"/>
       <c r="H16" s="3"/>
     </row>
-    <row r="17" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:11" x14ac:dyDescent="0.3">
       <c r="B17" s="5">
         <v>14</v>
       </c>
@@ -865,7 +874,7 @@
       <c r="G17" s="3"/>
       <c r="H17" s="3"/>
     </row>
-    <row r="18" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:11" x14ac:dyDescent="0.3">
       <c r="B18" s="5">
         <v>15</v>
       </c>
@@ -878,12 +887,12 @@
       <c r="G18" s="3"/>
       <c r="H18" s="3"/>
     </row>
-    <row r="20" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:11" x14ac:dyDescent="0.3">
       <c r="B20" s="9" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:11" x14ac:dyDescent="0.3">
       <c r="B21" s="2" t="s">
         <v>1</v>
       </c>
@@ -903,7 +912,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="22" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:11" x14ac:dyDescent="0.3">
       <c r="B22" s="5">
         <v>1</v>
       </c>
@@ -917,7 +926,7 @@
       <c r="F22" s="3"/>
       <c r="G22" s="3"/>
     </row>
-    <row r="23" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:11" x14ac:dyDescent="0.3">
       <c r="B23" s="5">
         <v>2</v>
       </c>
@@ -931,7 +940,7 @@
       <c r="F23" s="3"/>
       <c r="G23" s="3"/>
     </row>
-    <row r="24" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:11" x14ac:dyDescent="0.3">
       <c r="B24" s="5">
         <v>3</v>
       </c>
@@ -945,12 +954,13 @@
       <c r="F24" s="3"/>
       <c r="G24" s="3"/>
     </row>
-    <row r="29" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A29" s="10"/>
       <c r="B29" s="9" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="30" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:11" x14ac:dyDescent="0.3">
       <c r="B30" s="2" t="s">
         <v>1</v>
       </c>
@@ -982,7 +992,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="31" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:11" x14ac:dyDescent="0.3">
       <c r="B31" s="2">
         <v>1</v>
       </c>
@@ -1004,7 +1014,7 @@
       </c>
       <c r="K31" s="3"/>
     </row>
-    <row r="32" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:11" x14ac:dyDescent="0.3">
       <c r="B32" s="2">
         <v>2</v>
       </c>
@@ -1449,12 +1459,12 @@
         <v>18</v>
       </c>
     </row>
-    <row r="66" spans="2:8" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:8" x14ac:dyDescent="0.3">
       <c r="B66" s="9" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="67" spans="2:8" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:8" x14ac:dyDescent="0.3">
       <c r="B67" s="4" t="s">
         <v>1</v>
       </c>
@@ -1477,12 +1487,13 @@
         <v>25</v>
       </c>
     </row>
-    <row r="68" spans="2:8" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:8" x14ac:dyDescent="0.3">
       <c r="E68" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="80" spans="2:8" x14ac:dyDescent="0.3">
+    <row r="80" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A80" s="11"/>
       <c r="B80" s="9" t="s">
         <v>67</v>
       </c>

</xml_diff>